<commit_message>
fix validation is date
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fullstack\WebDev\googolplex-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802AE9D4-7A23-4F4E-8DD8-1DC7FEEA75DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC82A8F-26ED-4D9D-BCE9-CC07BBCBE2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E5DCAF38-FBE1-470E-8259-B5C753B95D38}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>endpoint</t>
   </si>
@@ -285,6 +285,59 @@
   </si>
   <si>
     <t>article</t>
+  </si>
+  <si>
+    <t>https://ecos.joheee.com/googolplex/article</t>
+  </si>
+  <si>
+    <t>{
+  "title": "this is article title",
+  "content": "this is article content"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "status": 200,
+  "message": "article with title this is article title is successfully created!",
+  "data": {
+    "id": "68cdbf11-a175-4487-a78a-8402261ec869",
+    "title": "this is article title",
+    "content": "this is article content"
+  }
+}</t>
+  </si>
+  <si>
+    <t>https://ecos.joheee.com/googolplex/article/68cdbf11-a175-4487-a78a-8402261ec869</t>
+  </si>
+  <si>
+    <t>{
+  "title": "this is update article title",
+  "content": "this is update article content"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "status": 200,
+  "message": "article is successfully updated!",
+  "data": {
+    "id": "68cdbf11-a175-4487-a78a-8402261ec869",
+    "title": "this is update article title",
+    "content": "this is update article content"
+  }
+}</t>
+  </si>
+  <si>
+    <t>assignment</t>
+  </si>
+  <si>
+    <t>https://ecos.joheee.com/googolplex/assignment</t>
+  </si>
+  <si>
+    <t>{
+  "title": "this is assignment title",
+  "content": "this is assignment content",
+  "due_date": "2024-12-31T23:59:59.999Z"
+}</t>
   </si>
 </sst>
 </file>
@@ -699,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0E90E5-D8E0-4F54-9565-07696B6F33FE}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,9 +949,58 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -907,8 +1009,11 @@
     <hyperlink ref="B7" r:id="rId2" xr:uid="{3AFB43D5-1867-43E6-9D4A-DC67AD86CB12}"/>
     <hyperlink ref="B8" r:id="rId3" xr:uid="{83B77A53-8AA0-405E-9582-E87E708B521C}"/>
     <hyperlink ref="B9" r:id="rId4" xr:uid="{59BE0D53-E658-4EC3-AC5F-73ECA51032AF}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{33746574-4A90-4DBE-89E8-BD7FEDABD16D}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{191BA809-D4C6-45E1-9003-6DA969E23405}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{7331327E-2682-41E5-B955-6A0B6CDDBFBA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix validation is number
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fullstack\WebDev\googolplex-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC82A8F-26ED-4D9D-BCE9-CC07BBCBE2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3E85DD-2E93-487D-ACEF-BB8B51AD965C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E5DCAF38-FBE1-470E-8259-B5C753B95D38}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>endpoint</t>
   </si>
@@ -338,6 +338,113 @@
   "content": "this is assignment content",
   "due_date": "2024-12-31T23:59:59.999Z"
 }</t>
+  </si>
+  <si>
+    <t>{
+  "status": 200,
+  "message": "assignment with title this is assignment title is successfully created!",
+  "data": {
+    "id": "5aa3b902-4b66-4080-bcb1-63f9d9cd86cc",
+    "title": "this is assignment title",
+    "content": "this is assignment content",
+    "due_date": "2024-12-31T23:59:59.999Z"
+  }
+}</t>
+  </si>
+  <si>
+    <t>https://ecos.joheee.com/googolplex/assignment/5aa3b902-4b66-4080-bcb1-63f9d9cd86cc</t>
+  </si>
+  <si>
+    <t>{
+  "title": "this is update title",
+  "content": "this is update content",
+  "due_date": "2025-01-30T23:59:59.999Z"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "status": 200,
+  "message": "assignment is successfully updated!",
+  "data": {
+    "id": "5aa3b902-4b66-4080-bcb1-63f9d9cd86cc",
+    "title": "this is update title",
+    "content": "this is update content",
+    "due_date": "2025-01-30T23:59:59.999Z"
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  "status": 200,
+  "message": "post successfully created!",
+  "data": {
+    "id": "825ebc07-3fa5-4753-a834-dad7ab0dd4b8",
+    "created_at": "2024-12-04T22:02:26.877Z",
+    "updated_at": "2024-12-04T22:02:26.877Z",
+    "article_id": "68cdbf11-a175-4487-a78a-8402261ec869",
+    "assignment_id": "5aa3b902-4b66-4080-bcb1-63f9d9cd86cc",
+    "class_id": "67d76221-4785-4d6d-a18e-0e19fb4fde30",
+    "article": {
+      "id": "68cdbf11-a175-4487-a78a-8402261ec869",
+      "title": "this is update article title",
+      "content": "this is update article content"
+    },
+    "assignment": {
+      "id": "5aa3b902-4b66-4080-bcb1-63f9d9cd86cc",
+      "title": "this is update title",
+      "content": "this is update content",
+      "due_date": "2025-01-30T23:59:59.999Z"
+    },
+    "class": {
+      "id": "67d76221-4785-4d6d-a18e-0e19fb4fde30",
+      "class_code": "VGSS6005",
+      "subject": "this is updated class subject",
+      "description": "this is updated class description",
+      "created_at": "2024-12-04T21:30:54.221Z",
+      "updated_at": "2024-12-04T21:33:00.137Z"
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>https://ecos.joheee.com/googolplex/post</t>
+  </si>
+  <si>
+    <t>{
+  "article_id": "68cdbf11-a175-4487-a78a-8402261ec869",
+  "assignment_id": "5aa3b902-4b66-4080-bcb1-63f9d9cd86cc",
+  "class_id": "67d76221-4785-4d6d-a18e-0e19fb4fde30"
+}</t>
+  </si>
+  <si>
+    <t>user_post_comment</t>
+  </si>
+  <si>
+    <t>https://ecos.joheee.com/googolplex/user_post_comment</t>
+  </si>
+  <si>
+    <t>{
+  "user_id": "a3383d40-1b5c-4355-8889-1aa84b0e61f7",
+  "post_id": "825ebc07-3fa5-4753-a834-dad7ab0dd4b8",
+  "comment": "this is post comment"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "status": 200,
+  "message": "user_post_comment successfully created!",
+  "data": {
+    "id": "63c28193-6ae7-4be9-ab1d-aa0b8e5c4885",
+    "created_at": "2024-12-04T22:04:27.702Z",
+    "updated_at": "2024-12-04T22:04:27.702Z",
+    "comment": "this is post comment",
+    "user_id": "a3383d40-1b5c-4355-8889-1aa84b0e61f7",
+    "post_id": "825ebc07-3fa5-4753-a834-dad7ab0dd4b8"
+  }
+}</t>
+  </si>
+  <si>
+    <t>user_assignment_todo</t>
   </si>
 </sst>
 </file>
@@ -752,15 +859,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0E90E5-D8E0-4F54-9565-07696B6F33FE}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="88.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="52" style="3" customWidth="1"/>
@@ -989,7 +1096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -1001,6 +1108,77 @@
       </c>
       <c r="D12" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1012,8 +1190,11 @@
     <hyperlink ref="B10" r:id="rId5" xr:uid="{33746574-4A90-4DBE-89E8-BD7FEDABD16D}"/>
     <hyperlink ref="B11" r:id="rId6" xr:uid="{191BA809-D4C6-45E1-9003-6DA969E23405}"/>
     <hyperlink ref="B12" r:id="rId7" xr:uid="{7331327E-2682-41E5-B955-6A0B6CDDBFBA}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{19BAA8D8-E0C7-42CC-8568-C23E0C467772}"/>
+    <hyperlink ref="B14" r:id="rId9" xr:uid="{9F7930D9-1A11-4E82-B05E-085DA66750BE}"/>
+    <hyperlink ref="B15" r:id="rId10" xr:uid="{2ADEA148-2F7E-4277-8D02-A3194610154E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>